<commit_message>
1. Ajuste na decodificação de mensagens 2. Adição de lista de veículos detectados
</commit_message>
<xml_diff>
--- a/AuxDox/Decodificador_mensagem_V00_R00.xlsx
+++ b/AuxDox/Decodificador_mensagem_V00_R00.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\favero.santos\PycharmProjects\ME\AuxDox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E380DB86-B3CF-4C8C-8AD3-1BD36F2F92C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9338B721-CCAE-4E88-82DE-8A6C78E62E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CAA23727-E135-465E-AFAF-7EAF40409B97}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{CAA23727-E135-465E-AFAF-7EAF40409B97}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="OBJECT_DATA" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
   <si>
     <t>B0</t>
   </si>
@@ -178,6 +179,12 @@
   </si>
   <si>
     <t>Index do python</t>
+  </si>
+  <si>
+    <t>dec</t>
+  </si>
+  <si>
+    <t>hex</t>
   </si>
 </sst>
 </file>
@@ -610,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF4DB46-9A25-4720-B80E-5438581550A7}">
   <dimension ref="A1:BM31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="B5:I7"/>
+    <sheetView topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P6" sqref="J5:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4030,4 +4037,85 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1992D2DD-F4D2-4C46-9986-EAFE2A42C05F}">
+  <dimension ref="B4:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>144</v>
+      </c>
+      <c r="D4">
+        <v>57</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>31</v>
+      </c>
+      <c r="G4">
+        <v>227</v>
+      </c>
+      <c r="H4">
+        <v>252</v>
+      </c>
+      <c r="I4">
+        <v>36</v>
+      </c>
+      <c r="J4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="str">
+        <f>DEC2HEX(C4)</f>
+        <v>90</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" ref="D5:J5" si="0">DEC2HEX(D4)</f>
+        <v>39</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>1F</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>E3</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>FC</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>A6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>